<commit_message>
add warning when temperature out of range
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.8.xlsx
+++ b/server/corelib/lang/all_lang_V1.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4A6D45-0D58-45E3-AC25-3AEBA6CE05B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4CA437-CDB9-4B91-814B-2AB8AFB7861F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="1205">
   <si>
     <t>name</t>
   </si>
@@ -3938,6 +3938,60 @@
   </si>
   <si>
     <t>温控箱IP</t>
+  </si>
+  <si>
+    <t>run_batchstats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>預估時間與溫度範圍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Approx. ranges of time and temperature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ca.. Bereiche von Zeit und Temperatur</t>
+  </si>
+  <si>
+    <t>预估时间与温度范围</t>
+  </si>
+  <si>
+    <t>exceed_max_temp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>exceed_min_temp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximun temperature is out of range</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum temperature is out of range</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>超過最大溫度上限</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>超過最小溫度下限</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximun Temperatur des Bereichs aus</t>
+  </si>
+  <si>
+    <t>超过最大温度上限</t>
+  </si>
+  <si>
+    <t>Tiefsttemperatur ist Bereich aus</t>
+  </si>
+  <si>
+    <t>超过最小温度下限</t>
   </si>
 </sst>
 </file>
@@ -4040,7 +4094,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="61">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4965,10 +5039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F259"/>
+  <dimension ref="A1:F262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" topLeftCell="A237" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D253" sqref="D253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6858,7 +6932,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>584</v>
@@ -6878,7 +6952,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>585</v>
@@ -6898,7 +6972,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>570</v>
@@ -6918,7 +6992,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>49</v>
@@ -6938,7 +7012,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>50</v>
@@ -6958,7 +7032,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>51</v>
@@ -6978,7 +7052,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>52</v>
@@ -6998,7 +7072,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>53</v>
@@ -7018,7 +7092,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>54</v>
@@ -7038,7 +7112,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>55</v>
@@ -7058,7 +7132,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>56</v>
@@ -7078,7 +7152,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>57</v>
@@ -7098,7 +7172,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>58</v>
@@ -7118,7 +7192,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>59</v>
@@ -7138,7 +7212,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>60</v>
@@ -7158,7 +7232,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>61</v>
@@ -7178,7 +7252,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>62</v>
@@ -7198,7 +7272,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>63</v>
@@ -7218,7 +7292,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>64</v>
@@ -7238,7 +7312,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>65</v>
@@ -7258,7 +7332,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>66</v>
@@ -7278,7 +7352,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>67</v>
@@ -7298,7 +7372,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>68</v>
@@ -7318,7 +7392,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>69</v>
@@ -7338,7 +7412,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>70</v>
@@ -7358,7 +7432,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>71</v>
@@ -7378,7 +7452,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>72</v>
@@ -7398,7 +7472,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>73</v>
@@ -7418,7 +7492,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>74</v>
@@ -7438,7 +7512,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>75</v>
@@ -7458,7 +7532,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>76</v>
@@ -7478,7 +7552,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>77</v>
@@ -7498,7 +7572,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>78</v>
@@ -7518,7 +7592,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>79</v>
@@ -7538,7 +7612,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>80</v>
@@ -7558,7 +7632,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>81</v>
@@ -7578,7 +7652,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>82</v>
@@ -7598,7 +7672,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>83</v>
@@ -7618,7 +7692,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>84</v>
@@ -7638,7 +7712,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>85</v>
@@ -7658,7 +7732,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>86</v>
@@ -7678,7 +7752,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>87</v>
@@ -7698,7 +7772,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>88</v>
@@ -7718,7 +7792,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>89</v>
@@ -7738,7 +7812,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>90</v>
@@ -7758,7 +7832,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>91</v>
@@ -7778,7 +7852,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>92</v>
@@ -7798,7 +7872,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>93</v>
@@ -7818,7 +7892,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>94</v>
@@ -7838,7 +7912,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>95</v>
@@ -7858,7 +7932,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>96</v>
@@ -7878,7 +7952,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>97</v>
@@ -7898,7 +7972,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>98</v>
@@ -7918,7 +7992,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>99</v>
@@ -7938,7 +8012,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>100</v>
@@ -7958,7 +8032,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>514</v>
@@ -7978,7 +8052,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>516</v>
@@ -7998,7 +8072,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>515</v>
@@ -8018,7 +8092,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>519</v>
@@ -8038,7 +8112,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>101</v>
@@ -8058,7 +8132,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>102</v>
@@ -8078,7 +8152,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>103</v>
@@ -8098,7 +8172,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>104</v>
@@ -8118,7 +8192,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>105</v>
@@ -8138,7 +8212,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>106</v>
@@ -8158,7 +8232,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>107</v>
@@ -8178,7 +8252,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>108</v>
@@ -8198,7 +8272,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>109</v>
@@ -8218,7 +8292,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>110</v>
@@ -8238,7 +8312,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>487</v>
@@ -8258,7 +8332,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>490</v>
@@ -8278,7 +8352,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>498</v>
@@ -8298,7 +8372,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>499</v>
@@ -8318,7 +8392,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>495</v>
@@ -8338,7 +8412,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>496</v>
@@ -8358,7 +8432,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>979</v>
@@ -8378,7 +8452,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>503</v>
@@ -8398,7 +8472,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>504</v>
@@ -8418,7 +8492,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>521</v>
@@ -8438,7 +8512,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>522</v>
@@ -8458,7 +8532,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>737</v>
@@ -8478,7 +8552,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>526</v>
@@ -8498,7 +8572,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>529</v>
@@ -8518,7 +8592,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>530</v>
@@ -8538,7 +8612,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>605</v>
@@ -8558,7 +8632,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>676</v>
@@ -8578,7 +8652,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>606</v>
@@ -8598,7 +8672,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>607</v>
@@ -8618,7 +8692,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>608</v>
@@ -8638,7 +8712,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>609</v>
@@ -8658,7 +8732,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>610</v>
@@ -8678,7 +8752,7 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>611</v>
@@ -8698,7 +8772,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>612</v>
@@ -8718,7 +8792,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>906</v>
@@ -8738,7 +8812,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>613</v>
@@ -8758,7 +8832,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>614</v>
@@ -8778,7 +8852,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>615</v>
@@ -8798,7 +8872,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>616</v>
@@ -8818,7 +8892,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>617</v>
@@ -8838,7 +8912,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>618</v>
@@ -8858,7 +8932,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>1024</v>
@@ -8878,7 +8952,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>619</v>
@@ -8898,7 +8972,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>620</v>
@@ -8918,7 +8992,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>621</v>
@@ -8938,7 +9012,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>622</v>
@@ -8958,7 +9032,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>623</v>
@@ -8978,7 +9052,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>624</v>
@@ -8998,7 +9072,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>625</v>
@@ -9018,7 +9092,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>626</v>
@@ -9038,7 +9112,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>627</v>
@@ -9058,7 +9132,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>628</v>
@@ -9078,7 +9152,7 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>908</v>
@@ -9098,7 +9172,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>907</v>
@@ -9118,7 +9192,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>684</v>
@@ -9138,7 +9212,7 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>683</v>
@@ -9158,7 +9232,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>974</v>
@@ -9178,7 +9252,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>909</v>
@@ -9198,7 +9272,7 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>910</v>
@@ -9218,7 +9292,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>1040</v>
@@ -9238,7 +9312,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>919</v>
@@ -9258,7 +9332,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>918</v>
@@ -9278,7 +9352,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>929</v>
@@ -9298,7 +9372,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>932</v>
@@ -9318,7 +9392,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>933</v>
@@ -9338,7 +9412,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>941</v>
@@ -9358,7 +9432,7 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>945</v>
@@ -9378,7 +9452,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>950</v>
@@ -9398,7 +9472,7 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>948</v>
@@ -9418,7 +9492,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>951</v>
@@ -9438,7 +9512,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>954</v>
@@ -9458,7 +9532,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>965</v>
@@ -9478,7 +9552,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>970</v>
@@ -9498,7 +9572,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>987</v>
@@ -9518,7 +9592,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>990</v>
@@ -9538,7 +9612,7 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>993</v>
@@ -9558,7 +9632,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>1029</v>
@@ -9578,7 +9652,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>1030</v>
@@ -9598,7 +9672,7 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>998</v>
@@ -9618,7 +9692,7 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>999</v>
@@ -9638,7 +9712,7 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>1000</v>
@@ -9658,7 +9732,7 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>1016</v>
@@ -9678,7 +9752,7 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>1031</v>
@@ -9698,7 +9772,7 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>1044</v>
@@ -9718,7 +9792,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>1045</v>
@@ -9738,7 +9812,7 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>1046</v>
@@ -9758,7 +9832,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>1058</v>
@@ -9778,7 +9852,7 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>1062</v>
@@ -9798,7 +9872,7 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>1067</v>
@@ -9818,7 +9892,7 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>1069</v>
@@ -9838,7 +9912,7 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>1070</v>
@@ -9858,7 +9932,7 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>1071</v>
@@ -9878,7 +9952,7 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>1072</v>
@@ -9898,7 +9972,7 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>1073</v>
@@ -9918,7 +9992,7 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>1081</v>
@@ -9938,7 +10012,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>1082</v>
@@ -9958,7 +10032,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>1083</v>
@@ -9978,7 +10052,7 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>1097</v>
@@ -9998,7 +10072,7 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>1124</v>
@@ -10018,7 +10092,7 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>1125</v>
@@ -10038,7 +10112,7 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>1126</v>
@@ -10058,7 +10132,7 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>1080</v>
@@ -10078,7 +10152,7 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>1127</v>
@@ -10098,7 +10172,7 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>1128</v>
@@ -10118,7 +10192,7 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>1136</v>
@@ -10138,7 +10212,7 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>1141</v>
@@ -10156,299 +10230,369 @@
         <v>1145</v>
       </c>
     </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" s="2">
+        <v>259</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="2">
+        <v>260</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D261" s="6" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="2">
+        <v>261</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>1204</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E155 B97:E152 B69:E72 B5:E6 B17:E29 B179:E200 B211:D211 B217:E218 B75:E84 B257:E258 D253:E253 C243:E248 B260:E1048576 B259:C259 B8:E14 B7:D7 B15:D15 B31:E38 B30:D30 B40:E46 B39:D39 B48:E66 B47:D47 B86:E89 B85:D85 B157:E159 B156:D156 B161:E161 B160:D160 B164:E166 B162:D163 B202:E205 B201:D201 B207:E207 B206:D206 B214:D216 B220:E220 B219:D219 B222:E222 B221:D221 B224:E225 B223:D223 B227:E230 B226:D226 B233:E233 B231:D232 B235:E235 B234:D234 B237:E241 B236:D236 C242:D242 C250:E251 C249:D249 D252 D256:E256 D254:D255">
+  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E155 B97:E152 B69:E72 B5:E6 B17:E29 B179:E200 B211:D211 B217:E218 B75:E84 B257:E258 D253:E253 C243:E248 B259:C259 B8:E14 B7:D7 B15:D15 B31:E38 B30:D30 B40:E46 B39:D39 B48:E66 B47:D47 B86:E89 B85:D85 B157:E159 B156:D156 B161:E161 B160:D160 B164:E166 B162:D163 B202:E205 B201:D201 B207:E207 B206:D206 B214:D216 B220:E220 B219:D219 B222:E222 B221:D221 B224:E225 B223:D223 B227:E230 B226:D226 B233:E233 B231:D232 B235:E235 B234:D234 B237:E241 B236:D236 C242:D242 C250:E251 C249:D249 D252 D256:E256 D254:D255 B260 B261:E1048576">
+    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B167:E167">
+    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B171:E172">
     <cfRule type="cellIs" dxfId="58" priority="61" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B167:E167">
+  <conditionalFormatting sqref="B153:D153">
     <cfRule type="cellIs" dxfId="57" priority="60" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B171:E172">
+  <conditionalFormatting sqref="B173:D173 B174 D174:E174">
     <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B153:D153">
+  <conditionalFormatting sqref="B175:E175 B176 D176">
     <cfRule type="cellIs" dxfId="55" priority="58" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B173:D173 B174 D174:E174">
+  <conditionalFormatting sqref="B177:E177 B178:D178">
     <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B175:E175 B176 D176">
+  <conditionalFormatting sqref="C176">
     <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B177:E177 B178:D178">
+  <conditionalFormatting sqref="C174">
     <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C176">
+  <conditionalFormatting sqref="B90:E90">
     <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C174">
+  <conditionalFormatting sqref="B91:D93">
     <cfRule type="cellIs" dxfId="50" priority="53" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:E90">
+  <conditionalFormatting sqref="E91:E92">
     <cfRule type="cellIs" dxfId="49" priority="52" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:D93">
+  <conditionalFormatting sqref="B94:D94 B96:D96">
     <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E92">
+  <conditionalFormatting sqref="E96">
     <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:D94 B96:D96">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="46" priority="49" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
+  <conditionalFormatting sqref="B67:E68">
     <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
+  <conditionalFormatting sqref="B208:E209">
     <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:E68">
+  <conditionalFormatting sqref="B73:D74">
     <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B208:E209">
+  <conditionalFormatting sqref="E74">
     <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:D74">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
+  <conditionalFormatting sqref="B16:D16">
     <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:D16">
+  <conditionalFormatting sqref="B207:E207">
     <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93">
+  <conditionalFormatting sqref="B206:D206">
     <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B207:E207">
+  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F66 F179:F207 F211 F214:F258 F261:F1048576">
     <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B206:D206">
+  <conditionalFormatting sqref="F167">
     <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F66 F179:F207 F211 F214:F258 F260:F1048576">
+  <conditionalFormatting sqref="F171:F172">
     <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F167">
+  <conditionalFormatting sqref="F153">
     <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F171:F172">
+  <conditionalFormatting sqref="F173:F174">
     <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F153">
+  <conditionalFormatting sqref="F175:F176">
     <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F173:F174">
+  <conditionalFormatting sqref="F177:F178">
     <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F175:F176">
+  <conditionalFormatting sqref="F90">
     <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F177:F178">
+  <conditionalFormatting sqref="F91:F93">
     <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90">
+  <conditionalFormatting sqref="F94 F96">
     <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:F93">
+  <conditionalFormatting sqref="F4">
     <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94 F96">
+  <conditionalFormatting sqref="F67:F68">
     <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="F208:F209">
     <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67:F68">
+  <conditionalFormatting sqref="F73:F74">
     <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F208:F209">
+  <conditionalFormatting sqref="F16">
     <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:F74">
+  <conditionalFormatting sqref="F207">
     <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
+  <conditionalFormatting sqref="F206">
     <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207">
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F206">
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B212:E212">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F212">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B210:E210">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F210">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B210:E210">
+  <conditionalFormatting sqref="B170:D170">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F210">
+  <conditionalFormatting sqref="F170">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B170:D170">
+  <conditionalFormatting sqref="B95:D95">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F170">
+  <conditionalFormatting sqref="E95">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B95:D95">
+  <conditionalFormatting sqref="F95">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95">
+  <conditionalFormatting sqref="B213:D213">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F95">
+  <conditionalFormatting sqref="F213">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B213:D213">
+  <conditionalFormatting sqref="C252:C256">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F213">
+  <conditionalFormatting sqref="B242:B251">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C252:C256">
+  <conditionalFormatting sqref="B252:B256">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B242:B251">
+  <conditionalFormatting sqref="E160">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B252:B256">
+  <conditionalFormatting sqref="D259:E259">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E160">
+  <conditionalFormatting sqref="F259">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D259:E259">
+  <conditionalFormatting sqref="E153">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F259">
+  <conditionalFormatting sqref="C260 E260">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E153">
+  <conditionalFormatting sqref="D260 F260">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix wording, add popout window after downloaded event data
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.8.xlsx
+++ b/server/corelib/lang/all_lang_V1.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56147F5-9103-4A2A-BBD7-E84BEC8C9AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC89CD90-DC7D-4678-AAAA-BE638F951946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="1248">
   <si>
     <t>name</t>
   </si>
@@ -3113,9 +3113,6 @@
     <t>流程准备程序</t>
   </si>
   <si>
-    <t>Sequence Teardown</t>
-  </si>
-  <si>
     <t>流程结束程序</t>
   </si>
   <si>
@@ -3529,10 +3526,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>loop id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>loop counts</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3851,9 +3844,6 @@
     <t>Anzahl der Messungen</t>
   </si>
   <si>
-    <t>Schleifen id</t>
-  </si>
-  <si>
     <t>Schleifen Farbe</t>
   </si>
   <si>
@@ -3901,9 +3891,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Ca.. Bereiche von Zeit und Temperatur</t>
-  </si>
-  <si>
     <t>预估时间与温度范围</t>
   </si>
   <si>
@@ -3947,10 +3934,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Go Teardown?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>teardown_error_title</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3967,10 +3950,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Go Teardown Step</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>流程結束程序</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3983,11 +3962,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Error During Test!
-Do you want to execute teardown step (heating process)?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>執行流程結束程序?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -4002,10 +3976,6 @@
     <t>执行流程结束程序?</t>
   </si>
   <si>
-    <t>Fehler beim Test!
-Wollen Sie Teardown Schritt (Heizprozess) auszuführen?</t>
-  </si>
-  <si>
     <t>发生错误! 是否要执行流程结束程序(加热程序)</t>
   </si>
   <si>
@@ -4040,18 +4010,6 @@
   </si>
   <si>
     <t>Test Stoppen</t>
-  </si>
-  <si>
-    <t>Sequenz Teardown</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Go Sequenz Teardown?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Go Sequenz Teardown</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>MearPos Guide</t>
@@ -4084,6 +4042,129 @@
   </si>
   <si>
     <t>请新增使用者权限后按下'新增'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sequence Shutdown procedure</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sequenz Abschalt Prozess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Go Abschalt Prozess?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Go Shutdown Procedure?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fehler beim Test!
+Wollen Sie Abschalt Prozess (Heizprozess) auszuführen?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error During Test!
+Do you want to execute Shutdown Procedure (heating process)?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Go Shutdown Procedure</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Go Abschalt Prozess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>settling_time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>settling time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>穩定時間</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Einschwingzeit</t>
+  </si>
+  <si>
+    <t>稳定时间</t>
+  </si>
+  <si>
+    <t>Ca. Bereiche von Zeit und Temperatur</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lower_letter_hard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lower_letter_temperature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lower_letter_humidity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hardness</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>humidity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>härte</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperatur</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>feuchtigkeit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lower_letter_time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>時間</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zeit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>等待时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>loop ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schleifen ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4223,23 +4304,113 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5184,10 +5355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F266"/>
+  <dimension ref="A1:F271"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A204" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D225" sqref="D225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5329,7 +5500,7 @@
         <v>580</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>739</v>
@@ -5489,7 +5660,7 @@
         <v>225</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>225</v>
@@ -5509,7 +5680,7 @@
         <v>697</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>744</v>
@@ -5783,16 +5954,16 @@
         <v>24</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="D30" s="12" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>1167</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>1170</v>
-      </c>
       <c r="F30" s="12" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -5803,16 +5974,16 @@
         <v>25</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -5969,7 +6140,7 @@
         <v>241</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>241</v>
@@ -6226,7 +6397,7 @@
         <v>150</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>1225</v>
+        <v>1214</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>345</v>
@@ -6246,13 +6417,13 @@
         <v>151</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1226</v>
+        <v>1215</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>346</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>1227</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -6889,7 +7060,7 @@
         <v>479</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>795</v>
@@ -6943,13 +7114,13 @@
         <v>443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>482</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F88" s="4" t="s">
         <v>798</v>
@@ -6963,16 +7134,16 @@
         <v>444</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>1208</v>
+        <v>1200</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -7049,7 +7220,7 @@
         <v>587</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>1224</v>
+        <v>1213</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>802</v>
@@ -7060,16 +7231,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>1027</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>1028</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>586</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="F94" s="4" t="s">
         <v>803</v>
@@ -7086,13 +7257,13 @@
         <v>583</v>
       </c>
       <c r="D95" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>1029</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="F95" s="4" t="s">
         <v>1030</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -7689,7 +7860,7 @@
         <v>279</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>1209</v>
+        <v>1201</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>825</v>
@@ -7789,7 +7960,7 @@
         <v>284</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>1210</v>
+        <v>1202</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>830</v>
@@ -8243,13 +8414,13 @@
         <v>516</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>517</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>1211</v>
+        <v>1203</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>852</v>
@@ -8309,7 +8480,7 @@
         <v>307</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>855</v>
@@ -8389,7 +8560,7 @@
         <v>311</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>1212</v>
+        <v>1204</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>859</v>
@@ -8429,7 +8600,7 @@
         <v>313</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>861</v>
@@ -8449,7 +8620,7 @@
         <v>314</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>862</v>
@@ -8503,16 +8674,16 @@
         <v>495</v>
       </c>
       <c r="C166" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="D166" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="D166" s="1" t="s">
+      <c r="E166" s="1" t="s">
         <v>977</v>
       </c>
-      <c r="E166" s="1" t="s">
+      <c r="F166" s="1" t="s">
         <v>978</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -8580,19 +8751,19 @@
         <v>169</v>
       </c>
       <c r="B170" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="C170" s="1" t="s">
         <v>972</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="D170" s="1" t="s">
         <v>973</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="E170" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F170" s="1" t="s">
         <v>974</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -8649,7 +8820,7 @@
         <v>521</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>870</v>
@@ -8709,7 +8880,7 @@
         <v>522</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>871</v>
@@ -8749,7 +8920,7 @@
         <v>522</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>871</v>
@@ -9080,19 +9251,19 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C195" s="1" t="s">
         <v>1017</v>
       </c>
-      <c r="C195" s="1" t="s">
+      <c r="D195" s="1" t="s">
         <v>1018</v>
       </c>
-      <c r="D195" s="1" t="s">
+      <c r="E195" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F195" s="1" t="s">
         <v>1019</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F195" s="1" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -9189,7 +9360,7 @@
         <v>662</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>1214</v>
+        <v>1206</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>794</v>
@@ -9209,7 +9380,7 @@
         <v>664</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>1215</v>
+        <v>1207</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>795</v>
@@ -9309,7 +9480,7 @@
         <v>730</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="F206" s="6" t="s">
         <v>899</v>
@@ -9380,19 +9551,19 @@
         <v>209</v>
       </c>
       <c r="B210" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="C210" s="1" t="s">
         <v>967</v>
       </c>
-      <c r="C210" s="1" t="s">
+      <c r="D210" s="4" t="s">
         <v>968</v>
       </c>
-      <c r="D210" s="4" t="s">
+      <c r="E210" s="3" t="s">
         <v>969</v>
       </c>
-      <c r="E210" s="3" t="s">
+      <c r="F210" s="4" t="s">
         <v>970</v>
-      </c>
-      <c r="F210" s="4" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -9409,7 +9580,7 @@
         <v>908</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="F211" s="4" t="s">
         <v>910</v>
@@ -9440,19 +9611,19 @@
         <v>212</v>
       </c>
       <c r="B213" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>1032</v>
       </c>
-      <c r="C213" s="1" t="s">
+      <c r="D213" s="4" t="s">
         <v>1033</v>
       </c>
-      <c r="D213" s="4" t="s">
+      <c r="E213" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F213" s="4" t="s">
         <v>1034</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>1150</v>
-      </c>
-      <c r="F213" s="4" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -9469,7 +9640,7 @@
         <v>917</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>918</v>
@@ -9489,7 +9660,7 @@
         <v>919</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>920</v>
@@ -9509,7 +9680,7 @@
         <v>925</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>926</v>
@@ -9569,7 +9740,7 @@
         <v>938</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>939</v>
@@ -9609,7 +9780,7 @@
         <v>952</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>953</v>
@@ -9623,16 +9794,16 @@
         <v>943</v>
       </c>
       <c r="C222" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F222" s="1" t="s">
         <v>954</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>1196</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>1216</v>
-      </c>
-      <c r="F222" s="1" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -9649,7 +9820,7 @@
         <v>244</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>763</v>
@@ -9666,10 +9837,10 @@
         <v>948</v>
       </c>
       <c r="D224" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="E224" s="1" t="s">
         <v>956</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>957</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>779</v>
@@ -9680,19 +9851,19 @@
         <v>224</v>
       </c>
       <c r="B225" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C225" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="C225" s="1" t="s">
+      <c r="D225" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="F225" s="1" t="s">
         <v>959</v>
-      </c>
-      <c r="D225" s="1" t="s">
-        <v>962</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>961</v>
-      </c>
-      <c r="F225" s="1" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -9700,19 +9871,19 @@
         <v>225</v>
       </c>
       <c r="B226" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="D226" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="C226" s="1" t="s">
-        <v>966</v>
-      </c>
-      <c r="D226" s="1" t="s">
+      <c r="E226" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F226" s="1" t="s">
         <v>964</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="F226" s="1" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -9720,19 +9891,19 @@
         <v>226</v>
       </c>
       <c r="B227" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="C227" s="1" t="s">
         <v>980</v>
       </c>
-      <c r="C227" s="1" t="s">
+      <c r="D227" s="6" t="s">
         <v>981</v>
       </c>
-      <c r="D227" s="6" t="s">
-        <v>982</v>
-      </c>
       <c r="E227" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="F227" s="1" t="s">
         <v>1000</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -9740,19 +9911,19 @@
         <v>227</v>
       </c>
       <c r="B228" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="C228" s="1" t="s">
         <v>983</v>
       </c>
-      <c r="C228" s="1" t="s">
+      <c r="D228" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="D228" s="1" t="s">
-        <v>985</v>
-      </c>
       <c r="E228" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F228" s="1" t="s">
         <v>1002</v>
-      </c>
-      <c r="F228" s="1" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -9760,19 +9931,19 @@
         <v>228</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C229" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="D229" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="D229" s="1" t="s">
-        <v>985</v>
-      </c>
       <c r="E229" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F229" s="1" t="s">
         <v>1002</v>
-      </c>
-      <c r="F229" s="1" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -9780,13 +9951,13 @@
         <v>229</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C230" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="D230" s="1" t="s">
         <v>987</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>988</v>
       </c>
       <c r="E230" s="1" t="s">
         <v>345</v>
@@ -9800,19 +9971,19 @@
         <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C231" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="D231" s="1" t="s">
         <v>989</v>
       </c>
-      <c r="D231" s="1" t="s">
-        <v>990</v>
-      </c>
       <c r="E231" s="1" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
@@ -9820,19 +9991,19 @@
         <v>231</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
@@ -9840,19 +10011,19 @@
         <v>232</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E233" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F233" s="1" t="s">
         <v>1006</v>
-      </c>
-      <c r="F233" s="1" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
@@ -9860,19 +10031,19 @@
         <v>233</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C234" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="D234" s="1" t="s">
         <v>996</v>
       </c>
-      <c r="D234" s="1" t="s">
-        <v>997</v>
-      </c>
       <c r="E234" s="1" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
@@ -9880,19 +10051,19 @@
         <v>234</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>440</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="E235" s="1" t="s">
         <v>326</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
@@ -9900,19 +10071,19 @@
         <v>235</v>
       </c>
       <c r="B236" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C236" s="1" t="s">
         <v>1023</v>
       </c>
-      <c r="C236" s="1" t="s">
+      <c r="D236" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F236" s="1" t="s">
         <v>1024</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>1026</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F236" s="1" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -9920,16 +10091,16 @@
         <v>236</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D237" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>741</v>
@@ -9940,19 +10111,19 @@
         <v>237</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E238" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F238" s="1" t="s">
         <v>1046</v>
-      </c>
-      <c r="F238" s="1" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
@@ -9960,19 +10131,19 @@
         <v>238</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E239" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F239" s="1" t="s">
         <v>1048</v>
-      </c>
-      <c r="F239" s="1" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
@@ -9980,19 +10151,19 @@
         <v>239</v>
       </c>
       <c r="B240" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C240" s="1" t="s">
         <v>1050</v>
       </c>
-      <c r="C240" s="1" t="s">
+      <c r="D240" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="D240" s="1" t="s">
+      <c r="E240" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F240" s="1" t="s">
         <v>1052</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F240" s="1" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
@@ -10000,19 +10171,19 @@
         <v>240</v>
       </c>
       <c r="B241" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C241" s="1" t="s">
         <v>1054</v>
       </c>
-      <c r="C241" s="1" t="s">
+      <c r="D241" s="1" t="s">
         <v>1055</v>
       </c>
-      <c r="D241" s="1" t="s">
+      <c r="E241" s="1" t="s">
         <v>1056</v>
       </c>
-      <c r="E241" s="1" t="s">
+      <c r="F241" s="1" t="s">
         <v>1057</v>
-      </c>
-      <c r="F241" s="1" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
@@ -10020,19 +10191,19 @@
         <v>241</v>
       </c>
       <c r="B242" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C242" s="1" t="s">
         <v>1059</v>
       </c>
-      <c r="C242" s="1" t="s">
-        <v>1060</v>
-      </c>
       <c r="D242" s="1" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
@@ -10040,19 +10211,19 @@
         <v>242</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
@@ -10060,19 +10231,19 @@
         <v>243</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
@@ -10080,19 +10251,19 @@
         <v>244</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
@@ -10100,19 +10271,19 @@
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
@@ -10120,19 +10291,19 @@
         <v>246</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
@@ -10140,19 +10311,19 @@
         <v>247</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="F248" s="1" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
@@ -10160,19 +10331,19 @@
         <v>248</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
@@ -10180,19 +10351,19 @@
         <v>249</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
@@ -10200,19 +10371,19 @@
         <v>250</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="C251" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D251" s="1" t="s">
         <v>1088</v>
       </c>
-      <c r="D251" s="1" t="s">
-        <v>1090</v>
-      </c>
       <c r="E251" s="1" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
@@ -10220,19 +10391,19 @@
         <v>251</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>1069</v>
+        <v>1246</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>1163</v>
+        <v>1247</v>
       </c>
       <c r="F252" s="1" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
@@ -10240,19 +10411,19 @@
         <v>252</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
@@ -10260,19 +10431,19 @@
         <v>253</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="F254" s="1" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
@@ -10280,19 +10451,19 @@
         <v>254</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>1221</v>
+        <v>1210</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
@@ -10300,19 +10471,19 @@
         <v>255</v>
       </c>
       <c r="B256" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C256" s="1" t="s">
         <v>1119</v>
       </c>
-      <c r="C256" s="1" t="s">
+      <c r="D256" s="6" t="s">
         <v>1121</v>
       </c>
-      <c r="D256" s="6" t="s">
+      <c r="E256" s="1" t="s">
         <v>1123</v>
       </c>
-      <c r="E256" s="1" t="s">
-        <v>1125</v>
-      </c>
       <c r="F256" s="1" t="s">
-        <v>1110</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
@@ -10320,504 +10491,649 @@
         <v>256</v>
       </c>
       <c r="B257" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C257" s="1" t="s">
         <v>1120</v>
       </c>
-      <c r="C257" s="1" t="s">
+      <c r="D257" s="1" t="s">
         <v>1122</v>
       </c>
-      <c r="D257" s="1" t="s">
+      <c r="E257" s="1" t="s">
         <v>1124</v>
       </c>
-      <c r="E257" s="1" t="s">
+      <c r="F257" s="1" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2">
+        <v>257</v>
+      </c>
+      <c r="B258" s="15" t="s">
         <v>1126</v>
       </c>
-      <c r="F257" s="1" t="s">
+      <c r="C258" s="15" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D258" s="15" t="s">
         <v>1127</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="16">
-        <v>257</v>
-      </c>
-      <c r="B258" s="17" t="s">
-        <v>1128</v>
-      </c>
-      <c r="C258" s="17" t="s">
+      <c r="E258" s="15" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F258" s="15" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2">
+        <v>258</v>
+      </c>
+      <c r="B259" s="15" t="s">
         <v>1130</v>
       </c>
-      <c r="D258" s="17" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E258" s="17" t="s">
+      <c r="C259" s="15" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D259" s="15" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E259" s="15" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F259" s="15" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="14">
+        <v>259</v>
+      </c>
+      <c r="B260" s="15" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C260" s="15" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D260" s="15" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E260" s="15" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F260" s="15" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="14">
+        <v>260</v>
+      </c>
+      <c r="B261" s="15" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C261" s="15" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D261" s="16" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E261" s="15" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F261" s="15" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="14">
+        <v>261</v>
+      </c>
+      <c r="B262" s="15" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C262" s="15" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D262" s="15" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E262" s="15" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F262" s="15" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="14">
+        <v>262</v>
+      </c>
+      <c r="B263" s="15" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C263" s="15" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D263" s="15" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E263" s="15" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F263" s="15" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A264" s="14">
+        <v>263</v>
+      </c>
+      <c r="B264" s="15" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C264" s="17" t="s">
         <v>1222</v>
       </c>
-      <c r="F258" s="17" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="16">
-        <v>258</v>
-      </c>
-      <c r="B259" s="17" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C259" s="17" t="s">
-        <v>1133</v>
-      </c>
-      <c r="D259" s="17" t="s">
-        <v>1134</v>
-      </c>
-      <c r="E259" s="17" t="s">
+      <c r="D264" s="15" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E264" s="17" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F264" s="15" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="14">
+        <v>264</v>
+      </c>
+      <c r="B265" s="15" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C265" s="15" t="s">
         <v>1223</v>
       </c>
-      <c r="F259" s="17" t="s">
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="9">
-        <v>259</v>
-      </c>
-      <c r="B260" s="10" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C260" s="10" t="s">
-        <v>1176</v>
-      </c>
-      <c r="D260" s="10" t="s">
-        <v>1175</v>
-      </c>
-      <c r="E260" s="10" t="s">
-        <v>1177</v>
-      </c>
-      <c r="F260" s="10" t="s">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="9">
-        <v>260</v>
-      </c>
-      <c r="B261" s="10" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C261" s="10" t="s">
-        <v>1181</v>
-      </c>
-      <c r="D261" s="14" t="s">
-        <v>1183</v>
-      </c>
-      <c r="E261" s="10" t="s">
-        <v>1185</v>
-      </c>
-      <c r="F261" s="10" t="s">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="9">
-        <v>261</v>
-      </c>
-      <c r="B262" s="10" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C262" s="10" t="s">
-        <v>1182</v>
-      </c>
-      <c r="D262" s="10" t="s">
-        <v>1184</v>
-      </c>
-      <c r="E262" s="10" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F262" s="10" t="s">
+      <c r="D265" s="15" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E265" s="15" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F265" s="15" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="14">
+        <v>265</v>
+      </c>
+      <c r="B266" s="15" t="s">
         <v>1188</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="9">
-        <v>262</v>
-      </c>
-      <c r="B263" s="10" t="s">
+      <c r="C266" s="15" t="s">
         <v>1189</v>
       </c>
-      <c r="C263" s="10" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D263" s="10" t="s">
-        <v>1200</v>
-      </c>
-      <c r="E263" s="10" t="s">
-        <v>1217</v>
-      </c>
-      <c r="F263" s="10" t="s">
-        <v>1203</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A264" s="9">
-        <v>263</v>
-      </c>
-      <c r="B264" s="10" t="s">
-        <v>1191</v>
-      </c>
-      <c r="C264" s="15" t="s">
+      <c r="D266" s="15" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E266" s="15" t="s">
         <v>1199</v>
       </c>
-      <c r="D264" s="10" t="s">
-        <v>1198</v>
-      </c>
-      <c r="E264" s="15" t="s">
-        <v>1204</v>
-      </c>
-      <c r="F264" s="10" t="s">
-        <v>1205</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="9">
-        <v>264</v>
-      </c>
-      <c r="B265" s="10" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C265" s="10" t="s">
-        <v>1195</v>
-      </c>
-      <c r="D265" s="10" t="s">
-        <v>1197</v>
-      </c>
-      <c r="E265" s="10" t="s">
-        <v>1218</v>
-      </c>
-      <c r="F265" s="10" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="9">
-        <v>265</v>
-      </c>
-      <c r="B266" s="10" t="s">
-        <v>1193</v>
-      </c>
-      <c r="C266" s="10" t="s">
+      <c r="F266" s="15" t="s">
         <v>1194</v>
       </c>
-      <c r="D266" s="10" t="s">
-        <v>1202</v>
-      </c>
-      <c r="E266" s="10" t="s">
-        <v>1207</v>
-      </c>
-      <c r="F266" s="10" t="s">
-        <v>1201</v>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" s="14">
+        <v>266</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F267" s="1" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" s="14">
+        <v>267</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D268" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="E268" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F268" s="4" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" s="14">
+        <v>268</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D269" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="E269" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F269" s="4" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" s="14">
+        <v>269</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D270" s="4" t="s">
+        <v>968</v>
+      </c>
+      <c r="E270" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F270" s="4" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" s="14">
+        <v>270</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D271" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E271" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="F271" s="4" t="s">
+        <v>1245</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E155 B97:E152 B69:E72 B5:E6 B17:E29 B179:E194 B211:D211 B217:E218 B75:E84 B257:E257 D253:E253 C243:E248 B259:C259 B8:E14 B7:D7 B15:D15 B31:E38 B30:D30 B40:E46 B39:D39 B48:E66 B47:D47 B86:E88 B85:D85 B157:E159 B156:D156 B161:E161 B160:D160 B164:E166 B162:D163 B202:E205 B207:E207 B206:D206 B214:D216 B220:E220 B219:D219 B222:E222 B221:D221 B224:E225 B223:D223 B227:E230 B226:D226 B233:E233 B231:D232 B235:E235 B234:D234 B237:E239 B236:D236 C242:D242 C250:E251 C249:D249 D252 D256:E256 D254:D255 B260 B261:E1048576 B89:D89 B196:E199 B195:D195 B200:D201 B241:E241 B240:D240 B258:D258">
+  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E155 B97:E152 B69:E72 B5:E6 B17:E29 B179:E194 B211:D211 B217:E218 B75:E84 B257:E257 D253:E253 C243:E248 B259:C259 B8:E14 B7:D7 B15:D15 B31:E38 B30:D30 B40:E46 B39:D39 B48:E66 B47:D47 B86:E88 B85:D85 B157:E159 B156:D156 B161:E161 B160:D160 B164:E166 B162:D163 B202:E205 B207:E207 B206:D206 B214:D216 B220:E220 B219:D219 B222:E222 B221:D221 B224:E225 B223:D223 B227:E230 B226:D226 B233:E233 B231:D232 B235:E235 B234:D234 B237:E239 B236:D236 C242:D242 C250:E251 C249:D249 D252 D256:E256 D254:D255 B260 B261:E266 B89:D89 B196:E199 B195:D195 B200:D201 B241:E241 B240:D240 B258:D258 B272:E1048576">
+    <cfRule type="cellIs" dxfId="69" priority="73" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B167:E167">
+    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B171:E172">
+    <cfRule type="cellIs" dxfId="67" priority="71" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B153:D153">
+    <cfRule type="cellIs" dxfId="66" priority="70" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B173:D173 B174 D174:E174">
+    <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B175:E175 B176 D176">
+    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B177:E177 B178:D178">
+    <cfRule type="cellIs" dxfId="63" priority="67" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C176">
+    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C174">
+    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B90:E90">
     <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B167:E167">
+  <conditionalFormatting sqref="B91:D93">
     <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B171:E172">
+  <conditionalFormatting sqref="E91:E92">
     <cfRule type="cellIs" dxfId="58" priority="62" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B153:D153">
+  <conditionalFormatting sqref="B94:D94 B96:D96">
     <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B173:D173 B174 D174:E174">
+  <conditionalFormatting sqref="E96">
     <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B175:E175 B176 D176">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B177:E177 B178:D178">
+  <conditionalFormatting sqref="B67:E68">
     <cfRule type="cellIs" dxfId="54" priority="58" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C176">
+  <conditionalFormatting sqref="B208:E209">
     <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C174">
+  <conditionalFormatting sqref="B73:D74">
     <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:E90">
+  <conditionalFormatting sqref="E74">
     <cfRule type="cellIs" dxfId="51" priority="55" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:D93">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E92">
+  <conditionalFormatting sqref="B16:D16">
     <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:D94 B96:D96">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
+  <conditionalFormatting sqref="B207:E207">
     <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
+  <conditionalFormatting sqref="B206:D206">
     <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:E68">
+  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F66 F179:F207 F211 F214:F258 F261:F266 F272:F1048576">
     <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B208:E209">
+  <conditionalFormatting sqref="F167">
     <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:D74">
+  <conditionalFormatting sqref="F171:F172">
     <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
+  <conditionalFormatting sqref="F153">
     <cfRule type="cellIs" dxfId="42" priority="46" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="F173:F174">
     <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:D16">
+  <conditionalFormatting sqref="F175:F176">
     <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93">
+  <conditionalFormatting sqref="F177:F178">
     <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B207:E207">
+  <conditionalFormatting sqref="F90">
     <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B206:D206">
+  <conditionalFormatting sqref="F91:F93">
     <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F66 F179:F207 F211 F214:F258 F261:F1048576">
+  <conditionalFormatting sqref="F94 F96">
     <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F167">
+  <conditionalFormatting sqref="F4">
     <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F171:F172">
+  <conditionalFormatting sqref="F67:F68">
     <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F153">
+  <conditionalFormatting sqref="F208:F209">
     <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F173:F174">
+  <conditionalFormatting sqref="F73:F74">
     <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F175:F176">
+  <conditionalFormatting sqref="F16">
     <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F177:F178">
+  <conditionalFormatting sqref="F207">
     <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90">
+  <conditionalFormatting sqref="F206">
     <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:F93">
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F94 F96">
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F67:F68">
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F208:F209">
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F73:F74">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F207">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F206">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B212:E212">
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F212">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B210:E210">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F210">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B170:D170">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F170">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B95:D95">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E95">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F95">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B213:D213">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F213">
     <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B210:E210">
+  <conditionalFormatting sqref="C252:C256">
     <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F210">
+  <conditionalFormatting sqref="B242:B251">
     <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B170:D170">
+  <conditionalFormatting sqref="B252:B256">
     <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F170">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+  <conditionalFormatting sqref="D259">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B95:D95">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+  <conditionalFormatting sqref="F259">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+  <conditionalFormatting sqref="E153">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F95">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+  <conditionalFormatting sqref="C260 E260">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B213:D213">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+  <conditionalFormatting sqref="D260 F260">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F213">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+  <conditionalFormatting sqref="E160">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C252:C256">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+  <conditionalFormatting sqref="C267:D267">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B242:B251">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+  <conditionalFormatting sqref="F267">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B252:B256">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+  <conditionalFormatting sqref="B267">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D259">
+  <conditionalFormatting sqref="B268:E269">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F259">
+  <conditionalFormatting sqref="F268:F269">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E153">
+  <conditionalFormatting sqref="B270:E270">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C260 E260">
+  <conditionalFormatting sqref="F270">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D260 F260">
+  <conditionalFormatting sqref="B271:E271">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E160">
+  <conditionalFormatting sqref="F271">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>